<commit_message>
Finished changes for release v1.0; Sept 19
</commit_message>
<xml_diff>
--- a/src/Packaging_Data.xlsx
+++ b/src/Packaging_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdyck\OneDrive\Documents\AIONEX SOLUTIONS\Longboard\Shipping_Packing_Optimizing_Project\Optimizer\Optimizer SW 250918\_internal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0551F8E2-BFAF-4228-AFAB-40F95030D67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0986A5F1-C736-462E-9805-CAEC3F818EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="10650" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packaging_Data" sheetId="5" r:id="rId1"/>
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -245,7 +245,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,28 +550,28 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" customWidth="1"/>
+    <col min="5" max="5" width="20.59765625" customWidth="1"/>
+    <col min="6" max="6" width="20.86328125" customWidth="1"/>
+    <col min="7" max="7" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.86328125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -606,9 +605,8 @@
       <c r="K1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,7 +617,7 @@
         <v>75</v>
       </c>
       <c r="D2" s="5">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="E2" s="8">
         <v>1.3605442176870748</v>
@@ -631,23 +629,22 @@
         <v>4</v>
       </c>
       <c r="H2" s="3">
-        <f>E2*G2</f>
+        <f t="shared" ref="H2:H12" si="0">E2*G2</f>
         <v>5.4421768707482991</v>
       </c>
       <c r="I2" s="10">
-        <f t="shared" ref="I2:I12" si="0">F2*2</f>
+        <f t="shared" ref="I2:I11" si="1">F2*2</f>
         <v>7320</v>
       </c>
       <c r="J2" s="10">
         <v>8</v>
       </c>
       <c r="K2" s="11">
-        <f>J2*E2</f>
+        <f t="shared" ref="K2:K12" si="2">J2*E2</f>
         <v>10.884353741496598</v>
       </c>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -670,23 +667,22 @@
         <v>1</v>
       </c>
       <c r="H3" s="3">
-        <f>E3*G3</f>
+        <f t="shared" si="0"/>
         <v>1.8095238095238095</v>
       </c>
       <c r="I3" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7320</v>
       </c>
       <c r="J3" s="10">
         <v>2</v>
       </c>
       <c r="K3" s="11">
-        <f>J3*E3</f>
+        <f t="shared" si="2"/>
         <v>3.6190476190476191</v>
       </c>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -709,23 +705,22 @@
         <v>1</v>
       </c>
       <c r="H4" s="3">
-        <f>E4*G4</f>
+        <f t="shared" si="0"/>
         <v>2.2675736961451247</v>
       </c>
       <c r="I4" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7320</v>
       </c>
       <c r="J4" s="10">
         <v>2</v>
       </c>
       <c r="K4" s="11">
-        <f>J4*E4</f>
+        <f t="shared" si="2"/>
         <v>4.5351473922902494</v>
       </c>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -733,12 +728,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="5">
-        <f>1*25.4</f>
-        <v>25.4</v>
+        <v>89</v>
       </c>
       <c r="D5" s="5">
-        <f>4*25.4</f>
-        <v>101.6</v>
+        <v>19</v>
       </c>
       <c r="E5" s="8">
         <v>0.49886621315192747</v>
@@ -751,23 +744,22 @@
         <v>2</v>
       </c>
       <c r="H5" s="3">
-        <f>E5*G5</f>
+        <f t="shared" si="0"/>
         <v>0.99773242630385495</v>
       </c>
       <c r="I5" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>965.19999999999993</v>
       </c>
       <c r="J5" s="10">
         <v>4</v>
       </c>
       <c r="K5" s="11">
-        <f>J5*E5</f>
+        <f t="shared" si="2"/>
         <v>1.9954648526077099</v>
       </c>
-      <c r="L5" s="14"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -775,12 +767,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="5">
-        <f>2*25.4</f>
-        <v>50.8</v>
+        <v>64</v>
       </c>
       <c r="D6" s="5">
-        <f>3*25.4</f>
-        <v>76.199999999999989</v>
+        <v>38</v>
       </c>
       <c r="E6" s="8">
         <v>0.89795918367346939</v>
@@ -793,23 +783,22 @@
         <v>2</v>
       </c>
       <c r="H6" s="3">
-        <f>E6*G6</f>
+        <f t="shared" si="0"/>
         <v>1.7959183673469388</v>
       </c>
       <c r="I6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>965.19999999999993</v>
       </c>
       <c r="J6" s="10">
         <v>4</v>
       </c>
       <c r="K6" s="11">
-        <f>J6*E6</f>
+        <f t="shared" si="2"/>
         <v>3.5918367346938775</v>
       </c>
-      <c r="L6" s="14"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -817,12 +806,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="5">
-        <f>1*25.4</f>
-        <v>25.4</v>
+        <v>89</v>
       </c>
       <c r="D7" s="5">
-        <f>3*25.4</f>
-        <v>76.199999999999989</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8">
         <v>2.7210884353741496</v>
@@ -834,23 +821,22 @@
         <v>1</v>
       </c>
       <c r="H7" s="3">
-        <f>E7*G7</f>
+        <f t="shared" si="0"/>
         <v>2.7210884353741496</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7320</v>
       </c>
       <c r="J7" s="10">
         <v>2</v>
       </c>
       <c r="K7" s="11">
-        <f>J7*E7</f>
+        <f t="shared" si="2"/>
         <v>5.4421768707482991</v>
       </c>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -875,23 +861,22 @@
         <v>2</v>
       </c>
       <c r="H8" s="3">
-        <f>E8*G8</f>
+        <f t="shared" si="0"/>
         <v>0.89795918367346939</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7320</v>
       </c>
       <c r="J8" s="10">
         <v>4</v>
       </c>
       <c r="K8" s="11">
-        <f>J8*E8</f>
+        <f t="shared" si="2"/>
         <v>1.7959183673469388</v>
       </c>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -903,7 +888,7 @@
         <v>254</v>
       </c>
       <c r="D9" s="6">
-        <f t="shared" ref="D9:D13" si="1">0.125*25.4</f>
+        <f t="shared" ref="D9:D13" si="3">0.125*25.4</f>
         <v>3.1749999999999998</v>
       </c>
       <c r="E9" s="8">
@@ -916,23 +901,22 @@
         <v>2</v>
       </c>
       <c r="H9" s="3">
-        <f>E9*G9</f>
+        <f t="shared" si="0"/>
         <v>1.9954648526077099</v>
       </c>
       <c r="I9" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7320</v>
       </c>
       <c r="J9" s="10">
         <v>4</v>
       </c>
       <c r="K9" s="11">
-        <f>J9*E9</f>
+        <f t="shared" si="2"/>
         <v>3.9909297052154198</v>
       </c>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -944,7 +928,7 @@
         <v>330.2</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.1749999999999998</v>
       </c>
       <c r="E10" s="8">
@@ -957,23 +941,22 @@
         <v>2</v>
       </c>
       <c r="H10" s="3">
-        <f>E10*G10</f>
+        <f t="shared" si="0"/>
         <v>1.9954648526077099</v>
       </c>
       <c r="I10" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7320</v>
       </c>
       <c r="J10" s="10">
         <v>4</v>
       </c>
       <c r="K10" s="11">
-        <f>J10*E10</f>
+        <f t="shared" si="2"/>
         <v>3.9909297052154198</v>
       </c>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -985,7 +968,7 @@
         <v>482.59999999999997</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.1749999999999998</v>
       </c>
       <c r="E11" s="8">
@@ -998,23 +981,22 @@
         <v>2</v>
       </c>
       <c r="H11" s="3">
-        <f>E11*G11</f>
+        <f t="shared" si="0"/>
         <v>2.7210884353741496</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7320</v>
       </c>
       <c r="J11" s="10">
         <v>4</v>
       </c>
       <c r="K11" s="11">
-        <f>J11*E11</f>
+        <f t="shared" si="2"/>
         <v>5.4421768707482991</v>
       </c>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1026,7 +1008,7 @@
         <v>482.59999999999997</v>
       </c>
       <c r="D12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.1749999999999998</v>
       </c>
       <c r="E12" s="8">
@@ -1039,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="3">
-        <f>E12*G12</f>
+        <f t="shared" si="0"/>
         <v>2.2675736961451247</v>
       </c>
       <c r="I12" s="10">
@@ -1050,12 +1032,11 @@
         <v>4</v>
       </c>
       <c r="K12" s="11">
-        <f>J12*E12</f>
+        <f t="shared" si="2"/>
         <v>4.5351473922902494</v>
       </c>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1067,7 +1048,7 @@
         <v>482.59999999999997</v>
       </c>
       <c r="D13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.1749999999999998</v>
       </c>
       <c r="E13" s="8">
@@ -1092,9 +1073,8 @@
       <c r="K13" s="10">
         <v>1</v>
       </c>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>

</xml_diff>